<commit_message>
preparing to release 0.0.6-pre; all countries added (but w/o much content)
also ideologies fixed
</commit_message>
<xml_diff>
--- a/План работ.xlsx
+++ b/План работ.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Krizhownik\Documents\Paradox Interactive\Hearts of Iron IV\mod\bofanski_ik\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D17334-8A3D-4380-83B1-7B50EE6591D6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2E28631-E72A-4560-A359-EA9C735FA95C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{29C851F8-096B-4DAA-81C4-84A9592ED549}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Государство</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>Почти готово</t>
+  </si>
+  <si>
+    <t>ЭЛОНГАЛ</t>
   </si>
 </sst>
 </file>
@@ -548,7 +551,7 @@
   <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,12 +612,8 @@
       <c r="B2" s="3">
         <v>2</v>
       </c>
-      <c r="C2" s="4">
-        <v>0</v>
-      </c>
-      <c r="D2" s="4">
-        <v>0</v>
-      </c>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
       <c r="E2" s="3">
         <v>1</v>
       </c>
@@ -659,12 +658,8 @@
       <c r="B4" s="21">
         <v>10</v>
       </c>
-      <c r="C4" s="4">
-        <v>0</v>
-      </c>
-      <c r="D4" s="4">
-        <v>0</v>
-      </c>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
       <c r="E4" s="12">
         <v>7</v>
       </c>
@@ -683,15 +678,11 @@
       <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="4">
-        <v>0</v>
-      </c>
-      <c r="C5" s="4">
-        <v>0</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0</v>
-      </c>
+      <c r="B5" s="9">
+        <v>20</v>
+      </c>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
       <c r="E5" s="12">
         <v>6</v>
       </c>
@@ -713,12 +704,8 @@
       <c r="B6" s="4">
         <v>0</v>
       </c>
-      <c r="C6" s="4">
-        <v>0</v>
-      </c>
-      <c r="D6" s="4">
-        <v>0</v>
-      </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
       <c r="E6" s="12">
         <v>5</v>
       </c>
@@ -740,12 +727,8 @@
       <c r="B7" s="4">
         <v>0</v>
       </c>
-      <c r="C7" s="4">
-        <v>0</v>
-      </c>
-      <c r="D7" s="4">
-        <v>0</v>
-      </c>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
       <c r="E7" s="12">
         <v>3</v>
       </c>
@@ -761,6 +744,23 @@
       <c r="P7" s="8"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0</v>
+      </c>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="12">
+        <v>2</v>
+      </c>
+      <c r="F8" s="12"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
       <c r="O8" s="17" t="s">
         <v>25</v>
       </c>

</xml_diff>